<commit_message>
begin work on TOD-S norms
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODC_adult_10.28.21_for norms/nwr_sum-adult-raw-ss-lookup-tabbed-age.xlsx
+++ b/OUTPUT-FILES/NORMS/TODC_adult_10.28.21_for norms/nwr_sum-adult-raw-ss-lookup-tabbed-age.xlsx
@@ -379,7 +379,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3">
@@ -387,7 +387,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
@@ -395,7 +395,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -403,7 +403,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">
@@ -411,7 +411,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7">
@@ -419,7 +419,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8">
@@ -427,7 +427,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9">
@@ -443,7 +443,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
@@ -451,7 +451,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12">
@@ -459,7 +459,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13">
@@ -467,7 +467,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14">
@@ -483,7 +483,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16">
@@ -491,7 +491,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17">
@@ -499,7 +499,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18">
@@ -507,7 +507,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19">
@@ -515,7 +515,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20">
@@ -523,7 +523,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21">
@@ -531,7 +531,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22">
@@ -539,7 +539,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23">
@@ -547,7 +547,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24">
@@ -555,7 +555,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25">
@@ -563,7 +563,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26">
@@ -571,7 +571,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27">
@@ -579,7 +579,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28">
@@ -587,7 +587,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29">
@@ -595,7 +595,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30">
@@ -603,7 +603,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31">
@@ -611,7 +611,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32">
@@ -619,7 +619,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33">
@@ -627,7 +627,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34">
@@ -635,7 +635,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35">
@@ -643,7 +643,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36">
@@ -651,7 +651,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37">
@@ -659,7 +659,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38">
@@ -667,7 +667,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39">
@@ -675,7 +675,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40">
@@ -691,7 +691,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42">
@@ -699,7 +699,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43">
@@ -715,7 +715,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45">
@@ -723,7 +723,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46">
@@ -731,7 +731,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47">
@@ -739,7 +739,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48">
@@ -747,7 +747,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>117</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49">
@@ -755,7 +755,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>119</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -788,7 +788,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3">
@@ -796,7 +796,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
@@ -804,7 +804,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -812,7 +812,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">
@@ -820,7 +820,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7">
@@ -828,7 +828,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8">
@@ -836,7 +836,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9">
@@ -852,7 +852,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
@@ -860,7 +860,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12">
@@ -868,7 +868,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13">
@@ -876,7 +876,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14">
@@ -884,7 +884,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
@@ -892,7 +892,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16">
@@ -900,7 +900,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17">
@@ -908,7 +908,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18">
@@ -916,7 +916,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19">
@@ -924,7 +924,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20">
@@ -932,7 +932,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21">
@@ -940,7 +940,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22">
@@ -948,7 +948,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23">
@@ -956,7 +956,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24">
@@ -972,7 +972,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26">
@@ -980,7 +980,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27">
@@ -988,7 +988,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28">
@@ -996,7 +996,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29">
@@ -1028,7 +1028,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33">
@@ -1036,7 +1036,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34">
@@ -1044,7 +1044,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35">
@@ -1052,7 +1052,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36">
@@ -1060,7 +1060,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37">
@@ -1068,7 +1068,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38">
@@ -1076,7 +1076,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39">
@@ -1084,7 +1084,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40">
@@ -1092,7 +1092,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41">
@@ -1100,7 +1100,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42">
@@ -1108,7 +1108,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43">
@@ -1116,7 +1116,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44">
@@ -1124,7 +1124,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45">
@@ -1132,7 +1132,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46">
@@ -1140,7 +1140,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47">
@@ -1148,7 +1148,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48">
@@ -1156,7 +1156,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49">
@@ -1164,7 +1164,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1197,7 +1197,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3">
@@ -1205,7 +1205,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
@@ -1213,7 +1213,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -1221,7 +1221,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">
@@ -1229,7 +1229,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7">
@@ -1237,7 +1237,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8">
@@ -1245,7 +1245,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9">
@@ -1261,7 +1261,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
@@ -1269,7 +1269,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12">
@@ -1277,7 +1277,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13">
@@ -1285,7 +1285,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14">
@@ -1293,7 +1293,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
@@ -1301,7 +1301,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16">
@@ -1309,7 +1309,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17">
@@ -1317,7 +1317,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18">
@@ -1325,7 +1325,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19">
@@ -1333,7 +1333,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20">
@@ -1341,7 +1341,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21">
@@ -1349,7 +1349,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22">
@@ -1357,7 +1357,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23">
@@ -1365,7 +1365,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24">
@@ -1373,7 +1373,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25">
@@ -1381,7 +1381,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26">
@@ -1389,7 +1389,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27">
@@ -1397,7 +1397,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28">
@@ -1405,7 +1405,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29">
@@ -1413,7 +1413,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30">
@@ -1421,7 +1421,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31">
@@ -1429,7 +1429,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32">
@@ -1437,7 +1437,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33">
@@ -1445,7 +1445,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34">
@@ -1453,7 +1453,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35">
@@ -1461,7 +1461,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36">
@@ -1469,7 +1469,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37">
@@ -1477,7 +1477,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38">
@@ -1485,7 +1485,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39">
@@ -1493,7 +1493,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>117</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40">
@@ -1501,7 +1501,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>117</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41">
@@ -1509,7 +1509,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>117</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42">
@@ -1517,7 +1517,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>117</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43">
@@ -1525,7 +1525,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>117</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44">
@@ -1533,7 +1533,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>117</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45">
@@ -1541,7 +1541,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46">
@@ -1549,7 +1549,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>117</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47">
@@ -1557,7 +1557,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>117</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48">
@@ -1565,7 +1565,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49">
@@ -1573,7 +1573,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1606,7 +1606,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3">
@@ -1614,7 +1614,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4">
@@ -1622,7 +1622,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -1630,7 +1630,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">
@@ -1638,7 +1638,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7">
@@ -1646,7 +1646,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8">
@@ -1670,7 +1670,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
@@ -1678,7 +1678,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12">
@@ -1686,7 +1686,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13">
@@ -1694,7 +1694,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14">
@@ -1702,7 +1702,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
@@ -1710,7 +1710,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16">
@@ -1718,7 +1718,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17">
@@ -1726,7 +1726,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18">
@@ -1734,7 +1734,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19">
@@ -1742,7 +1742,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20">
@@ -1750,7 +1750,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21">
@@ -1758,7 +1758,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22">
@@ -1766,7 +1766,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23">
@@ -1774,7 +1774,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24">
@@ -1782,7 +1782,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25">
@@ -1790,7 +1790,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26">
@@ -1798,7 +1798,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27">
@@ -1806,7 +1806,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28">
@@ -1814,7 +1814,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29">
@@ -1822,7 +1822,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30">
@@ -1830,7 +1830,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31">
@@ -1838,7 +1838,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32">
@@ -1846,7 +1846,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33">
@@ -1854,7 +1854,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34">
@@ -1862,7 +1862,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35">
@@ -1870,7 +1870,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36">
@@ -1878,7 +1878,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37">
@@ -1886,7 +1886,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38">
@@ -1894,7 +1894,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39">
@@ -1902,7 +1902,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>118</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40">
@@ -1910,7 +1910,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>118</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41">
@@ -1918,7 +1918,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>118</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42">
@@ -1926,7 +1926,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>118</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43">
@@ -1934,7 +1934,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>118</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44">
@@ -1942,7 +1942,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>118</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45">
@@ -1950,7 +1950,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>118</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46">
@@ -1958,7 +1958,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>121</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47">
@@ -1966,7 +1966,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>121</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48">
@@ -1974,7 +1974,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49">
@@ -1982,7 +1982,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2015,7 +2015,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3">
@@ -2023,7 +2023,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4">
@@ -2031,7 +2031,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5">
@@ -2039,7 +2039,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">
@@ -2047,7 +2047,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7">
@@ -2055,7 +2055,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8">
@@ -2071,7 +2071,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10">
@@ -2079,7 +2079,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
@@ -2087,7 +2087,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12">
@@ -2095,7 +2095,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13">
@@ -2103,7 +2103,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14">
@@ -2111,7 +2111,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15">
@@ -2119,7 +2119,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16">
@@ -2127,7 +2127,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17">
@@ -2135,7 +2135,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18">
@@ -2143,7 +2143,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19">
@@ -2151,7 +2151,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20">
@@ -2159,7 +2159,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21">
@@ -2167,7 +2167,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22">
@@ -2175,7 +2175,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23">
@@ -2183,7 +2183,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24">
@@ -2191,7 +2191,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25">
@@ -2199,7 +2199,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26">
@@ -2207,7 +2207,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27">
@@ -2215,7 +2215,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28">
@@ -2223,7 +2223,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29">
@@ -2231,7 +2231,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30">
@@ -2239,7 +2239,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31">
@@ -2247,7 +2247,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32">
@@ -2255,7 +2255,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33">
@@ -2263,7 +2263,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34">
@@ -2271,7 +2271,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35">
@@ -2279,7 +2279,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36">
@@ -2287,7 +2287,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37">
@@ -2295,7 +2295,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38">
@@ -2303,7 +2303,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>117</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39">
@@ -2311,7 +2311,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>117</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40">
@@ -2319,7 +2319,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>117</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41">
@@ -2327,7 +2327,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>117</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42">
@@ -2335,7 +2335,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>117</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43">
@@ -2343,7 +2343,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44">
@@ -2351,7 +2351,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45">
@@ -2359,7 +2359,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>117</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46">
@@ -2367,7 +2367,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>121</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47">
@@ -2375,7 +2375,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>121</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48">
@@ -2383,7 +2383,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>121</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49">
@@ -2391,7 +2391,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2424,7 +2424,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3">
@@ -2448,7 +2448,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6">
@@ -2456,7 +2456,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7">
@@ -2464,7 +2464,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8">
@@ -2472,7 +2472,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9">
@@ -2496,7 +2496,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12">
@@ -2504,7 +2504,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13">
@@ -2512,7 +2512,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14">
@@ -2520,7 +2520,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15">
@@ -2528,7 +2528,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16">
@@ -2536,7 +2536,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17">
@@ -2544,7 +2544,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18">
@@ -2552,7 +2552,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19">
@@ -2560,7 +2560,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20">
@@ -2568,7 +2568,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21">
@@ -2576,7 +2576,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22">
@@ -2584,7 +2584,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23">
@@ -2592,7 +2592,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24">
@@ -2600,7 +2600,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25">
@@ -2608,7 +2608,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26">
@@ -2616,7 +2616,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27">
@@ -2624,7 +2624,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28">
@@ -2632,7 +2632,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29">
@@ -2648,7 +2648,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31">
@@ -2656,7 +2656,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32">
@@ -2688,7 +2688,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36">
@@ -2696,7 +2696,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37">
@@ -2704,7 +2704,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38">
@@ -2712,7 +2712,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39">
@@ -2720,7 +2720,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40">
@@ -2728,7 +2728,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41">
@@ -2736,7 +2736,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42">
@@ -2744,7 +2744,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43">
@@ -2752,7 +2752,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44">
@@ -2760,7 +2760,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45">
@@ -2768,7 +2768,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46">
@@ -2776,7 +2776,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47">
@@ -2784,7 +2784,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48">
@@ -2792,7 +2792,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49">
@@ -2800,7 +2800,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>